<commit_message>
Quiz 2 and solutions
</commit_message>
<xml_diff>
--- a/MAN 4558 ~ Lean Operations/Quiz2.xlsx
+++ b/MAN 4558 ~ Lean Operations/Quiz2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guslipkin/Documents/GitHub/Spring2022/MAN 4558 ~ Lean Operations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF984339-5834-C441-9C6A-E61ECE32A6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F348F22C-5010-4D41-9D1B-284A14E3F98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="18000" windowHeight="22500" xr2:uid="{D8135C66-0532-44A2-A5F6-036075D10527}"/>
+    <workbookView xWindow="18000" yWindow="880" windowWidth="18000" windowHeight="22500" xr2:uid="{D8135C66-0532-44A2-A5F6-036075D10527}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E96B88-D41A-4529-91DD-43761C4E13AA}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -767,6 +767,10 @@
       <c r="P3">
         <v>386</v>
       </c>
+      <c r="R3">
+        <f xml:space="preserve"> B3 - P3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">

</xml_diff>